<commit_message>
Auto and Figure updates
</commit_message>
<xml_diff>
--- a/Tables/autocorr_stats.xlsx
+++ b/Tables/autocorr_stats.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel_anstett/Dropbox/a Papers/Rapid_drought/Paper 3/climate_lag/Tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{08246E70-6EA4-9D43-9EFB-1BB3AB881158}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCACD9FD-E8A3-E64E-B6F8-B8B503D4D028}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="autocorr_stats" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="10">
   <si>
     <t>slope</t>
   </si>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
@@ -562,7 +562,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -570,8 +570,6 @@
     <xf numFmtId="2" fontId="0" fillId="33" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -579,10 +577,19 @@
     <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="16" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="16" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -939,11 +946,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:O11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -952,8 +959,8 @@
     <col min="3" max="3" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="6"/>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A1" s="4"/>
       <c r="B1" s="9" t="s">
         <v>8</v>
       </c>
@@ -964,30 +971,60 @@
       </c>
       <c r="F1" s="9"/>
       <c r="G1" s="9"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="N1" s="9"/>
+      <c r="O1" s="9"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="5"/>
-      <c r="B2" s="10" t="s">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A2" s="3"/>
+      <c r="B2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="7" t="s">
         <v>2</v>
       </c>
+      <c r="I2" s="3"/>
+      <c r="J2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="O2" s="7" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="1">
@@ -1008,9 +1045,30 @@
       <c r="G3" s="1">
         <v>1.6169444698843399E-4</v>
       </c>
+      <c r="I3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3" s="10">
+        <v>-20.392776837848601</v>
+      </c>
+      <c r="K3" s="10">
+        <v>0.63813641287203904</v>
+      </c>
+      <c r="L3" s="10">
+        <v>2.2980390528202999E-2</v>
+      </c>
+      <c r="M3" s="10">
+        <v>2.04238338476909</v>
+      </c>
+      <c r="N3" s="10">
+        <v>0.96871367807854503</v>
+      </c>
+      <c r="O3" s="10">
+        <v>1.6169444698843399E-4</v>
+      </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="1">
@@ -1025,15 +1083,36 @@
       <c r="E4" s="1">
         <v>81.462676700244003</v>
       </c>
-      <c r="F4" s="11">
+      <c r="F4" s="8">
         <v>9.6255736405444395E-2</v>
       </c>
       <c r="G4" s="1">
         <v>0.252068997283383</v>
       </c>
+      <c r="I4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="J4" s="10">
+        <v>49.662210776883697</v>
+      </c>
+      <c r="K4" s="10">
+        <v>0.24275214442302501</v>
+      </c>
+      <c r="L4" s="10">
+        <v>0.13354827504775901</v>
+      </c>
+      <c r="M4" s="10">
+        <v>81.462676700244003</v>
+      </c>
+      <c r="N4" s="10">
+        <v>9.6255736405444395E-2</v>
+      </c>
+      <c r="O4" s="10">
+        <v>0.252068997283383</v>
+      </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="2">
@@ -1054,9 +1133,38 @@
       <c r="G5" s="2">
         <v>2.33872891147946E-5</v>
       </c>
+      <c r="I5" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="J5" s="10">
+        <v>-7.2142588972246298</v>
+      </c>
+      <c r="K5" s="10">
+        <v>0.876966489038429</v>
+      </c>
+      <c r="L5" s="10">
+        <v>2.5162749682394298E-3</v>
+      </c>
+      <c r="M5" s="10">
+        <v>0.83041401284743099</v>
+      </c>
+      <c r="N5" s="10">
+        <v>0.98809917733427799</v>
+      </c>
+      <c r="O5" s="10">
+        <v>2.33872891147946E-5</v>
+      </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="6"/>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
+      <c r="M6" s="10"/>
+      <c r="N6" s="10"/>
+      <c r="O6" s="10"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A7" s="4"/>
       <c r="B7" s="9" t="s">
         <v>6</v>
       </c>
@@ -1067,30 +1175,60 @@
       </c>
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="N7" s="11"/>
+      <c r="O7" s="11"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="5"/>
-      <c r="B8" s="10" t="s">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A8" s="3"/>
+      <c r="B8" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E8" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="F8" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="G8" s="10" t="s">
+      <c r="G8" s="7" t="s">
         <v>2</v>
       </c>
+      <c r="I8" s="3"/>
+      <c r="J8" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="K8" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="L8" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="M8" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="N8" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="O8" s="12" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="7" t="s">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B9" s="1">
@@ -1111,9 +1249,30 @@
       <c r="G9" s="1">
         <v>2.07458174729209E-2</v>
       </c>
+      <c r="I9" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="J9" s="10">
+        <v>-10.127146467964799</v>
+      </c>
+      <c r="K9" s="10">
+        <v>0.14235788074705999</v>
+      </c>
+      <c r="L9" s="10">
+        <v>0.20229989995070399</v>
+      </c>
+      <c r="M9" s="10">
+        <v>2.9242989736084701</v>
+      </c>
+      <c r="N9" s="10">
+        <v>0.65516457433513398</v>
+      </c>
+      <c r="O9" s="10">
+        <v>2.07458174729209E-2</v>
+      </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="7" t="s">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B10" s="1">
@@ -1134,9 +1293,30 @@
       <c r="G10" s="1">
         <v>6.7620000529420493E-2</v>
       </c>
+      <c r="I10" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="J10" s="10">
+        <v>7.5610730424014001</v>
+      </c>
+      <c r="K10" s="10">
+        <v>0.291099342992096</v>
+      </c>
+      <c r="L10" s="10">
+        <v>0.110501930788971</v>
+      </c>
+      <c r="M10" s="10">
+        <v>-5.3333897698581296</v>
+      </c>
+      <c r="N10" s="10">
+        <v>0.41435871239870198</v>
+      </c>
+      <c r="O10" s="10">
+        <v>6.7620000529420493E-2</v>
+      </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="8" t="s">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
         <v>5</v>
       </c>
       <c r="B11" s="2">
@@ -1157,13 +1337,38 @@
       <c r="G11" s="2">
         <v>4.71606433765306E-2</v>
       </c>
+      <c r="I11" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="J11" s="10">
+        <v>-11.167212057422899</v>
+      </c>
+      <c r="K11" s="10">
+        <v>0.12871509678073001</v>
+      </c>
+      <c r="L11" s="10">
+        <v>0.215219188904193</v>
+      </c>
+      <c r="M11" s="10">
+        <v>-4.7136937943747101</v>
+      </c>
+      <c r="N11" s="10">
+        <v>0.49778123237206501</v>
+      </c>
+      <c r="O11" s="10">
+        <v>4.71606433765306E-2</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="8">
+    <mergeCell ref="M1:O1"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="M7:O7"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="B7:D7"/>
     <mergeCell ref="E7:G7"/>
+    <mergeCell ref="J1:L1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>